<commit_message>
updated descriptions of measurements.
</commit_message>
<xml_diff>
--- a/Rooftop_Antenna_Measurements_August_10th/rooftop measurement description.xlsx
+++ b/Rooftop_Antenna_Measurements_August_10th/rooftop measurement description.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="13540" yWindow="0" windowWidth="11240" windowHeight="12740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -39,9 +39,6 @@
     <t>white cable with 50 ohm termination</t>
   </si>
   <si>
-    <t>White cable with short</t>
-  </si>
-  <si>
     <t>s11_black_cable_load</t>
   </si>
   <si>
@@ -81,47 +78,119 @@
     <t>white cable attached to N terminal of Cambridge balun not attached to antenna</t>
   </si>
   <si>
-    <t>Balun attached to cable at position 2</t>
-  </si>
-  <si>
-    <t>s11_cambridge_balun_N_ant_1</t>
-  </si>
-  <si>
-    <t>s11_cambridge_balun_N_ant_2</t>
-  </si>
-  <si>
-    <t>Balun attached to cable at position 1</t>
-  </si>
-  <si>
-    <t>s11_hybrid_balun_ant_AA</t>
-  </si>
-  <si>
-    <t>Balun attached to hybrid coupler balun, A,  port A.</t>
-  </si>
-  <si>
-    <t>s11_hybrid_balun_ant_AB</t>
-  </si>
-  <si>
-    <t>Balun attached to hybrid coupler balun A, port B.</t>
-  </si>
-  <si>
-    <t>s11_hybrid_balun_ant_BB</t>
-  </si>
-  <si>
-    <t>s11_hybrid_balun_ant_BA</t>
-  </si>
-  <si>
-    <t>Hybrid coupler B balun attached to white cable port B</t>
-  </si>
-  <si>
-    <t>Hybrid coupler B balun attached to white calbe port A</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Existence Verified</t>
+  </si>
+  <si>
+    <t>Additional Comments</t>
+  </si>
+  <si>
+    <t>s11_cambridge_balun_N_antenna_1</t>
+  </si>
+  <si>
+    <t>s11_cambridge_balun_N_antenna_0</t>
+  </si>
+  <si>
+    <t>Cambridge Balun attached to antenna pol-North</t>
+  </si>
+  <si>
+    <t>Cambridge Balun attached to antenna pol-North, cable moved</t>
+  </si>
+  <si>
+    <t>s11_hybrid_A_port_B_antenna</t>
+  </si>
+  <si>
+    <t>s11_hybrid_A_port_A_antenna</t>
+  </si>
+  <si>
+    <t>s11_hybrid_B_port_A_antenna</t>
+  </si>
+  <si>
+    <t>s11_hybrid_B_port_B_antenna</t>
+  </si>
+  <si>
+    <t>Hybrid coupler B balun attached antenna measured through white cable port B (common mode)</t>
+  </si>
+  <si>
+    <t>Hybrid coupler Balun A attached to antenna with NN through board. Measured through  white cable through port B (common mode)</t>
+  </si>
+  <si>
+    <t>Hybrid coupler balun, A attached to antenna North pol through board with,  measured with port A through white cable (differential mode).</t>
+  </si>
+  <si>
+    <t>Hybrid coupler B balun attached to antenna NN pol with through board and measured through white cable port A (common Mode).</t>
+  </si>
+  <si>
+    <t>s11_no_balun_antenna</t>
+  </si>
+  <si>
+    <t>s12_no_balun_antenna</t>
+  </si>
+  <si>
+    <t>s21_no_balun_antenna</t>
+  </si>
+  <si>
+    <t>s22_no_balun_antenna</t>
+  </si>
+  <si>
+    <t>differential measurement with no balun. Pol north white cable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">differential measurement with no balun. Pol north white cable </t>
+  </si>
+  <si>
+    <t>differential measurement with no balun. Pol north white cable</t>
+  </si>
+  <si>
+    <t>Relevant Picture</t>
+  </si>
+  <si>
+    <t>1881, 1882,1883</t>
+  </si>
+  <si>
+    <t>1878 1879 1880</t>
+  </si>
+  <si>
+    <t>1877, 1876,1875</t>
+  </si>
+  <si>
+    <t>1866, 1868, 1867</t>
+  </si>
+  <si>
+    <t>1874, 1873, 1872</t>
+  </si>
+  <si>
+    <t>1865,1864, 1863,1862</t>
+  </si>
+  <si>
+    <t>1857, 1858</t>
+  </si>
+  <si>
+    <t>White cable open</t>
+  </si>
+  <si>
+    <t>s11_hybrid_A_port_A</t>
+  </si>
+  <si>
+    <t>Hybrid coupler balun A measured through port A with white cable. Ports C/D open</t>
+  </si>
+  <si>
+    <t>s11_hybrid_A_port_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybrid coupler balun A measured through port B with white cable, C/D open. </t>
+  </si>
+  <si>
+    <t>1884, 1885</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +214,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,21 +239,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,15 +617,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,21 +638,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -547,117 +674,280 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>